<commit_message>
merged evaluate.py and wordseq_test.py
</commit_message>
<xml_diff>
--- a/report/pics/graphs_seq.xlsx
+++ b/report/pics/graphs_seq.xlsx
@@ -43,34 +43,34 @@
     <t xml:space="preserve">GRU</t>
   </si>
   <si>
-    <t xml:space="preserve">seq0+w2v_f100</t>
+    <t xml:space="preserve">seqv0+w2v_f100</t>
   </si>
   <si>
-    <t xml:space="preserve">seq0+w2v_f300</t>
+    <t xml:space="preserve">seqv0+w2v_f300</t>
   </si>
   <si>
-    <t xml:space="preserve">seq0+w2v_f600</t>
+    <t xml:space="preserve">seqv0+w2v_f600</t>
   </si>
   <si>
-    <t xml:space="preserve">seq0+w2v_bio02</t>
+    <t xml:space="preserve">seqv0+w2v_bio02</t>
   </si>
   <si>
-    <t xml:space="preserve">seq0+w2v_bio30</t>
+    <t xml:space="preserve">seqv0+w2v_bio30</t>
   </si>
   <si>
-    <t xml:space="preserve">seq1+w2v_f100</t>
+    <t xml:space="preserve">seqv1+w2v_f100</t>
   </si>
   <si>
-    <t xml:space="preserve">seq1+w2v_f300</t>
+    <t xml:space="preserve">seqv1+w2v_f300</t>
   </si>
   <si>
-    <t xml:space="preserve">seq1+w2v_f600</t>
+    <t xml:space="preserve">seqv1+w2v_f600</t>
   </si>
   <si>
-    <t xml:space="preserve">seq1+w2v_bio02</t>
+    <t xml:space="preserve">seqv1+w2v_bio02</t>
   </si>
   <si>
-    <t xml:space="preserve">seq1+w2v_bio30</t>
+    <t xml:space="preserve">seqv1+w2v_bio30</t>
   </si>
 </sst>
 </file>
@@ -248,7 +248,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -296,34 +296,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -406,34 +406,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -516,34 +516,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -590,11 +590,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="38327115"/>
-        <c:axId val="88987761"/>
+        <c:axId val="32757701"/>
+        <c:axId val="87468212"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38327115"/>
+        <c:axId val="32757701"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,14 +629,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88987761"/>
+        <c:crossAx val="87468212"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88987761"/>
+        <c:axId val="87468212"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -718,7 +718,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38327115"/>
+        <c:crossAx val="32757701"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -754,7 +754,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -802,34 +802,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -912,34 +912,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1022,34 +1022,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1096,11 +1096,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="28008864"/>
-        <c:axId val="18570100"/>
+        <c:axId val="28498340"/>
+        <c:axId val="69728361"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="28008864"/>
+        <c:axId val="28498340"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,14 +1135,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18570100"/>
+        <c:crossAx val="69728361"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18570100"/>
+        <c:axId val="69728361"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1224,7 +1224,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28008864"/>
+        <c:crossAx val="28498340"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1260,7 +1260,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1318,34 +1318,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1440,34 +1440,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1562,34 +1562,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1643,11 +1643,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="8709235"/>
-        <c:axId val="12074165"/>
+        <c:axId val="95900960"/>
+        <c:axId val="12097009"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8709235"/>
+        <c:axId val="95900960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1682,14 +1682,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12074165"/>
+        <c:crossAx val="12097009"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12074165"/>
+        <c:axId val="12097009"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1771,7 +1771,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8709235"/>
+        <c:crossAx val="95900960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1808,7 +1808,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1866,34 +1866,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1988,34 +1988,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2110,34 +2110,34 @@
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>seq0+w2v_f100</c:v>
+                  <c:v>seqv0+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>seq0+w2v_f300</c:v>
+                  <c:v>seqv0+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>seq0+w2v_f600</c:v>
+                  <c:v>seqv0+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>seq0+w2v_bio02</c:v>
+                  <c:v>seqv0+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>seq0+w2v_bio30</c:v>
+                  <c:v>seqv0+w2v_bio30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>seq1+w2v_f100</c:v>
+                  <c:v>seqv1+w2v_f100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>seq1+w2v_f300</c:v>
+                  <c:v>seqv1+w2v_f300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>seq1+w2v_f600</c:v>
+                  <c:v>seqv1+w2v_f600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>seq1+w2v_bio02</c:v>
+                  <c:v>seqv1+w2v_bio02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>seq1+w2v_bio30</c:v>
+                  <c:v>seqv1+w2v_bio30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2191,11 +2191,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="98027238"/>
-        <c:axId val="31446440"/>
+        <c:axId val="46206845"/>
+        <c:axId val="39063193"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98027238"/>
+        <c:axId val="46206845"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2230,14 +2230,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31446440"/>
+        <c:crossAx val="39063193"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31446440"/>
+        <c:axId val="39063193"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2319,7 +2319,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98027238"/>
+        <c:crossAx val="46206845"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2367,9 +2367,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>168480</xdr:colOff>
+      <xdr:colOff>168120</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>47160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2378,7 +2378,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="277560" y="2266200"/>
-        <a:ext cx="4719960" cy="2657880"/>
+        <a:ext cx="4719600" cy="2657520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2397,9 +2397,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>746280</xdr:colOff>
+      <xdr:colOff>745920</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2408,7 +2408,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5598000" y="2139120"/>
-        <a:ext cx="4854240" cy="2730240"/>
+        <a:ext cx="4853880" cy="2729880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2427,9 +2427,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>168120</xdr:colOff>
+      <xdr:colOff>167760</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2438,7 +2438,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="277200" y="5077440"/>
-        <a:ext cx="4719960" cy="2657880"/>
+        <a:ext cx="4719600" cy="2657520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2457,9 +2457,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
+      <xdr:colOff>2520</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2468,7 +2468,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5667120" y="5068080"/>
-        <a:ext cx="4854240" cy="2730240"/>
+        <a:ext cx="4853880" cy="2729880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2488,8 +2488,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>